<commit_message>
Bug 3111 final changes for release
</commit_message>
<xml_diff>
--- a/IosReleaseTesting.xlsx
+++ b/IosReleaseTesting.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1960" yWindow="660" windowWidth="38900" windowHeight="19160" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.2.0 1_26_2015" sheetId="1" r:id="rId4"/>
+    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="V1.2.1 6_9_2015" sheetId="1" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="35">
   <si>
     <t>Overall Test completion</t>
   </si>
@@ -124,11 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -145,17 +151,12 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -271,72 +272,72 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -344,29 +345,80 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="fff4f4f4"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFF4F4F4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -558,7 +610,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -567,7 +619,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -576,7 +628,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -585,7 +637,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -594,7 +646,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -603,7 +655,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -715,8 +767,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -724,14 +776,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -750,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +810,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -786,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -890,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -916,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -942,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,7 +1020,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -994,7 +1046,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,9 +1059,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1025,7 +1083,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1044,7 +1102,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1070,7 +1128,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1096,7 +1154,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1122,7 +1180,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1148,7 +1206,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1174,7 +1232,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1200,7 +1258,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1226,7 +1284,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1252,7 +1310,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1278,7 +1336,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,9 +1349,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1306,7 +1370,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1325,7 +1389,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1355,7 +1419,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1381,7 +1445,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1407,7 +1471,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,7 +1497,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,7 +1523,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1485,7 +1549,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1511,7 +1575,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1537,7 +1601,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1563,7 +1627,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1576,26 +1640,33 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
     <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
@@ -1605,18 +1676,12 @@
     <col min="6" max="6" width="5.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="56.7734" style="1" customWidth="1"/>
+    <col min="9" max="9" width="56.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="33.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.25" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.25" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.25" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.25" style="1" customWidth="1"/>
-    <col min="17" max="256" width="12.25" style="1" customWidth="1"/>
+    <col min="11" max="256" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8" customHeight="1">
+    <row r="1" spans="1:16" ht="8" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1634,7 +1699,7 @@
       <c r="O1" s="3"/>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" ht="20.55" customHeight="1">
+    <row r="2" spans="1:16" ht="20.5" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -1652,34 +1717,34 @@
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
     </row>
-    <row r="3" ht="32.55" customHeight="1">
+    <row r="3" spans="1:16" ht="32.5" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="8"/>
-      <c r="C3" t="s" s="9">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s" s="9">
+      <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s" s="9">
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s" s="9">
+      <c r="H3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s" s="9">
+      <c r="I3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s" s="9">
+      <c r="J3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s" s="9">
+      <c r="K3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="10"/>
@@ -1688,7 +1753,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" ht="20.35" customHeight="1">
+    <row r="4" spans="1:16" ht="20.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
@@ -1706,33 +1771,33 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" ht="22.35" customHeight="1">
+    <row r="5" spans="1:16" ht="22.25" customHeight="1">
       <c r="A5" s="5"/>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s" s="14">
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s" s="15">
+      <c r="I5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s" s="14">
+      <c r="J5" s="14" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="16"/>
@@ -1742,31 +1807,31 @@
       <c r="O5" s="16"/>
       <c r="P5" s="16"/>
     </row>
-    <row r="6" ht="20.35" customHeight="1">
+    <row r="6" spans="1:16" ht="20.25" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" t="s" s="13">
+      <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s" s="17">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s" s="17">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s" s="17">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s" s="17">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s" s="17">
+      <c r="C6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="18"/>
-      <c r="I6" t="s" s="17">
+      <c r="I6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J6" t="s" s="19">
+      <c r="J6" s="19" t="s">
         <v>16</v>
       </c>
       <c r="K6" s="12"/>
@@ -1776,25 +1841,25 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" ht="20.35" customHeight="1">
+    <row r="7" spans="1:16" ht="20.25" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="11"/>
-      <c r="C7" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s" s="14">
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
-      <c r="J7" t="s" s="14">
+      <c r="J7" s="14" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="16"/>
@@ -1804,27 +1869,27 @@
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
     </row>
-    <row r="8" ht="20.35" customHeight="1">
+    <row r="8" spans="1:16" ht="20.25" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="11"/>
-      <c r="C8" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s" s="19">
+      <c r="C8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="J8" t="s" s="19">
+      <c r="J8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="K8" s="12"/>
@@ -1834,27 +1899,27 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" ht="32.35" customHeight="1">
+    <row r="9" spans="1:16" ht="32.25" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="11"/>
-      <c r="C9" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s" s="14">
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
-      <c r="J9" t="s" s="14">
+      <c r="J9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="K9" s="16"/>
@@ -1864,31 +1929,31 @@
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
     </row>
-    <row r="10" ht="36.35" customHeight="1">
+    <row r="10" spans="1:16" ht="36.25" customHeight="1">
       <c r="A10" s="5"/>
-      <c r="B10" t="s" s="13">
+      <c r="B10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s" s="19">
+      <c r="C10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="12"/>
-      <c r="I10" t="s" s="17">
+      <c r="I10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s" s="19">
+      <c r="J10" s="19" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="12"/>
@@ -1898,27 +1963,27 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" ht="20.35" customHeight="1">
+    <row r="11" spans="1:16" ht="20.25" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="11"/>
-      <c r="C11" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s" s="14">
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
-      <c r="J11" t="s" s="14">
+      <c r="J11" s="14" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="16"/>
@@ -1928,27 +1993,27 @@
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
     </row>
-    <row r="12" ht="20.35" customHeight="1">
+    <row r="12" spans="1:16" ht="20.25" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="11"/>
-      <c r="C12" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s" s="19">
+      <c r="C12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
-      <c r="J12" t="s" s="19">
+      <c r="J12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="12"/>
@@ -1958,27 +2023,27 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" ht="20.35" customHeight="1">
+    <row r="13" spans="1:16" ht="20.25" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="11"/>
-      <c r="C13" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="G13" t="s" s="14">
+      <c r="C13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
-      <c r="J13" t="s" s="14">
+      <c r="J13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="16"/>
@@ -1988,31 +2053,31 @@
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
     </row>
-    <row r="14" ht="20.35" customHeight="1">
+    <row r="14" spans="1:16" ht="20.25" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" t="s" s="13">
+      <c r="B14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s" s="19">
+      <c r="C14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" t="s" s="17">
+      <c r="I14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J14" t="s" s="19">
+      <c r="J14" s="19" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="12"/>
@@ -2022,27 +2087,27 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" ht="20.35" customHeight="1">
+    <row r="15" spans="1:16" ht="20.25" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="11"/>
-      <c r="C15" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="G15" t="s" s="14">
+      <c r="C15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
-      <c r="J15" t="s" s="14">
+      <c r="J15" s="14" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="16"/>
@@ -2052,27 +2117,27 @@
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
     </row>
-    <row r="16" ht="37.4" customHeight="1">
+    <row r="16" spans="1:16" ht="37.5" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="11"/>
-      <c r="C16" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s" s="19">
-        <v>10</v>
-      </c>
-      <c r="G16" t="s" s="19">
+      <c r="C16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
-      <c r="J16" t="s" s="19">
+      <c r="J16" s="19" t="s">
         <v>27</v>
       </c>
       <c r="K16" s="12"/>
@@ -2082,27 +2147,27 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
     </row>
-    <row r="17" ht="20.35" customHeight="1">
+    <row r="17" spans="1:16" ht="20.25" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="11"/>
-      <c r="C17" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="G17" t="s" s="14">
+      <c r="C17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
-      <c r="J17" t="s" s="14">
+      <c r="J17" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K17" s="16"/>
@@ -2112,9 +2177,9 @@
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
     </row>
-    <row r="18" ht="53" customHeight="1">
+    <row r="18" spans="1:16" ht="53" customHeight="1">
       <c r="A18" s="5"/>
-      <c r="B18" t="s" s="13">
+      <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="12"/>
@@ -2122,13 +2187,13 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" t="s" s="19">
+      <c r="H18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I18" t="s" s="17">
+      <c r="I18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="J18" t="s" s="19">
+      <c r="J18" s="19" t="s">
         <v>31</v>
       </c>
       <c r="K18" s="12"/>
@@ -2138,12 +2203,12 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" ht="20.35" customHeight="1">
+    <row r="19" spans="1:16" ht="20.25" customHeight="1">
       <c r="A19" s="5"/>
-      <c r="B19" t="s" s="13">
+      <c r="B19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s" s="14">
+      <c r="C19" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="16"/>
@@ -2151,7 +2216,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" t="s" s="15">
+      <c r="I19" s="15" t="s">
         <v>33</v>
       </c>
       <c r="J19" s="16"/>
@@ -2162,10 +2227,10 @@
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
     </row>
-    <row r="20" ht="20.35" customHeight="1">
+    <row r="20" spans="1:16" ht="20.25" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="11"/>
-      <c r="C20" t="s" s="19">
+      <c r="C20" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="12"/>
@@ -2173,7 +2238,7 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="I20" t="s" s="15">
+      <c r="I20" s="15" t="s">
         <v>34</v>
       </c>
       <c r="J20" s="12"/>
@@ -2184,10 +2249,10 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" ht="20.35" customHeight="1">
+    <row r="21" spans="1:16" ht="20.25" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="11"/>
-      <c r="C21" t="s" s="14">
+      <c r="C21" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="16"/>
@@ -2195,7 +2260,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" t="s" s="17">
+      <c r="I21" s="17" t="s">
         <v>26</v>
       </c>
       <c r="J21" s="16"/>
@@ -2206,7 +2271,7 @@
       <c r="O21" s="16"/>
       <c r="P21" s="16"/>
     </row>
-    <row r="22" ht="20.35" customHeight="1">
+    <row r="22" spans="1:16" ht="20.25" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2224,7 +2289,7 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
     </row>
-    <row r="23" ht="20.35" customHeight="1">
+    <row r="23" spans="1:16" ht="20.25" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="11"/>
       <c r="C23" s="16"/>
@@ -2242,7 +2307,7 @@
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
     </row>
-    <row r="24" ht="20.35" customHeight="1">
+    <row r="24" spans="1:16" ht="20.25" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -2260,7 +2325,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" ht="20.35" customHeight="1">
+    <row r="25" spans="1:16" ht="20.25" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="11"/>
       <c r="C25" s="16"/>
@@ -2278,7 +2343,7 @@
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
     </row>
-    <row r="26" ht="20.35" customHeight="1">
+    <row r="26" spans="1:16" ht="20.25" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
@@ -2296,7 +2361,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
     </row>
-    <row r="27" ht="20.35" customHeight="1">
+    <row r="27" spans="1:16" ht="20.25" customHeight="1">
       <c r="A27" s="20"/>
       <c r="B27" s="11"/>
       <c r="C27" s="16"/>
@@ -2316,9 +2381,678 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:IV27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="1" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="56.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5" style="1" customWidth="1"/>
+    <col min="11" max="256" width="12.25" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="8" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" ht="32.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" ht="22.25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" ht="32.25" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" ht="36.25" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" ht="37.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+    </row>
+    <row r="18" spans="1:16" ht="53" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+    </row>
+    <row r="22" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+    </row>
+    <row r="25" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+    </row>
+    <row r="26" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+    </row>
+    <row r="27" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug 2781 V 1.2.2 updates - Added CoreData stuff
</commit_message>
<xml_diff>
--- a/IosReleaseTesting.xlsx
+++ b/IosReleaseTesting.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="660" windowWidth="38900" windowHeight="19160" activeTab="1"/>
+    <workbookView xWindow="1960" yWindow="660" windowWidth="38900" windowHeight="19160"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="V1.2.2 7_10_2015" sheetId="3" r:id="rId1"/>
     <sheet name="V1.2.1 6_9_2015" sheetId="1" r:id="rId2"/>
+    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="37">
   <si>
     <t>Overall Test completion</t>
   </si>
@@ -128,6 +129,12 @@
   </si>
   <si>
     <t>/Users/scoleman/dev/fips/fcids/release/V1.2.0_01_26_2015/testcordova.xcodeproj</t>
+  </si>
+  <si>
+    <t>/Users/scoleman/dev/fips/fcids/release/Vxxx.../fips-pi.xcodeproj</t>
+  </si>
+  <si>
+    <t>/Users/scoleman/dev/fips/fcids/release/Vxxx.../testcordova.xcodeproj</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1671,9 @@
   </sheetPr>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1779,18 +1788,10 @@
       <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
         <v>11</v>
       </c>
@@ -1812,9 +1813,7 @@
       <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>10</v>
-      </c>
+      <c r="C6" s="17"/>
       <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
@@ -1824,9 +1823,7 @@
       <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="17" t="s">
-        <v>10</v>
-      </c>
+      <c r="G6" s="17"/>
       <c r="H6" s="18"/>
       <c r="I6" s="17" t="s">
         <v>15</v>
@@ -1844,9 +1841,7 @@
     <row r="7" spans="1:16" ht="20.25" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
         <v>10</v>
       </c>
@@ -1872,9 +1867,7 @@
     <row r="8" spans="1:16" ht="20.25" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="C8" s="19"/>
       <c r="D8" s="19" t="s">
         <v>10</v>
       </c>
@@ -1884,9 +1877,7 @@
       <c r="F8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="G8" s="19"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="19" t="s">
@@ -1902,9 +1893,7 @@
     <row r="9" spans="1:16" ht="32.25" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
@@ -1914,9 +1903,7 @@
       <c r="F9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="G9" s="14"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="14" t="s">
@@ -1934,9 +1921,7 @@
       <c r="B10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1946,9 +1931,7 @@
       <c r="F10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="G10" s="19"/>
       <c r="H10" s="12"/>
       <c r="I10" s="17" t="s">
         <v>21</v>
@@ -1966,9 +1949,7 @@
     <row r="11" spans="1:16" ht="20.25" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
@@ -1978,9 +1959,7 @@
       <c r="F11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="G11" s="14"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="14" t="s">
@@ -1996,9 +1975,7 @@
     <row r="12" spans="1:16" ht="20.25" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="C12" s="19"/>
       <c r="D12" s="19" t="s">
         <v>10</v>
       </c>
@@ -2008,9 +1985,7 @@
       <c r="F12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="G12" s="19"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="19" t="s">
@@ -2026,9 +2001,7 @@
     <row r="13" spans="1:16" ht="20.25" customHeight="1">
       <c r="A13" s="5"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
@@ -2038,9 +2011,7 @@
       <c r="F13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="G13" s="14"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="14" t="s">
@@ -2058,21 +2029,11 @@
       <c r="B14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="12"/>
       <c r="I14" s="17" t="s">
         <v>26</v>
@@ -2090,21 +2051,11 @@
     <row r="15" spans="1:16" ht="20.25" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="14" t="s">
@@ -2120,21 +2071,11 @@
     <row r="16" spans="1:16" ht="37.5" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="19" t="s">
@@ -2150,21 +2091,11 @@
     <row r="17" spans="1:16" ht="20.25" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
       <c r="J17" s="14" t="s">
@@ -2208,16 +2139,14 @@
       <c r="B19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C19" s="14"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -2230,16 +2159,14 @@
     <row r="20" spans="1:16" ht="20.25" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="11"/>
-      <c r="C20" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="C20" s="19"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
@@ -2252,9 +2179,7 @@
     <row r="21" spans="1:16" ht="20.25" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C21" s="14"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -2400,7 +2325,7 @@
   </sheetPr>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -3055,4 +2980,740 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:IV27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="1" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="56.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5" style="1" customWidth="1"/>
+    <col min="11" max="256" width="12.25" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="8" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" ht="32.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" ht="22.25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" ht="32.25" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" ht="36.25" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" ht="37.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+    </row>
+    <row r="18" spans="1:16" ht="53" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+    </row>
+    <row r="22" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+    </row>
+    <row r="25" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+    </row>
+    <row r="26" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+    </row>
+    <row r="27" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug 2920 Updated docs
</commit_message>
<xml_diff>
--- a/IosReleaseTesting.xlsx
+++ b/IosReleaseTesting.xlsx
@@ -7,9 +7,10 @@
     <workbookView xWindow="1960" yWindow="660" windowWidth="38900" windowHeight="19160"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.2.2 7_10_2015" sheetId="3" r:id="rId1"/>
-    <sheet name="V1.2.1 6_9_2015" sheetId="1" r:id="rId2"/>
-    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="V1.2.3 7_31_201" sheetId="4" r:id="rId1"/>
+    <sheet name="V1.2.2 7_10_2015" sheetId="3" r:id="rId2"/>
+    <sheet name="V1.2.1 6_9_2015" sheetId="1" r:id="rId3"/>
+    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="38">
   <si>
     <t>Overall Test completion</t>
   </si>
@@ -135,6 +136,11 @@
   </si>
   <si>
     <t>/Users/scoleman/dev/fips/fcids/release/Vxxx.../testcordova.xcodeproj</t>
+  </si>
+  <si>
+    <t>Confirm release directory has necessary files + ex: /Users/scoleman/dev/fips/fcids/release/V1.2.0_01_26_2015 +Confirm no errors</t>
   </si>
 </sst>
 </file>
@@ -1672,7 +1678,7 @@
   <dimension ref="A1:IV27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="E6" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1817,9 +1823,7 @@
       <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>10</v>
-      </c>
+      <c r="E6" s="17"/>
       <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
@@ -1845,9 +1849,7 @@
       <c r="D7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
         <v>10</v>
       </c>
@@ -1871,9 +1873,7 @@
       <c r="D8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="19"/>
       <c r="F8" s="19" t="s">
         <v>10</v>
       </c>
@@ -1897,9 +1897,7 @@
       <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="E9" s="14"/>
       <c r="F9" s="14" t="s">
         <v>10</v>
       </c>
@@ -1922,15 +1920,9 @@
         <v>20</v>
       </c>
       <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="12"/>
       <c r="I10" s="17" t="s">
@@ -1950,15 +1942,9 @@
       <c r="A11" s="5"/>
       <c r="B11" s="11"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -1976,15 +1962,9 @@
       <c r="A12" s="5"/>
       <c r="B12" s="11"/>
       <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="19"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -2002,15 +1982,9 @@
       <c r="A13" s="5"/>
       <c r="B13" s="11"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -2125,7 +2099,7 @@
         <v>30</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -2319,6 +2293,660 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:IV27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="1" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="56.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5" style="1" customWidth="1"/>
+    <col min="11" max="256" width="12.25" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="8" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" ht="32.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" ht="22.25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" ht="32.25" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" ht="36.25" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" ht="37.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+    </row>
+    <row r="18" spans="1:16" ht="53" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+    </row>
+    <row r="22" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+    </row>
+    <row r="25" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+    </row>
+    <row r="26" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+    </row>
+    <row r="27" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
@@ -2982,7 +3610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
Bug 2781 - Minor file fixes
</commit_message>
<xml_diff>
--- a/IosReleaseTesting.xlsx
+++ b/IosReleaseTesting.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="660" windowWidth="38900" windowHeight="19160"/>
+    <workbookView xWindow="4320" yWindow="140" windowWidth="36760" windowHeight="20240"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.2.3 7_31_201" sheetId="4" r:id="rId1"/>
-    <sheet name="V1.2.2 7_10_2015" sheetId="3" r:id="rId2"/>
-    <sheet name="V1.2.1 6_9_2015" sheetId="1" r:id="rId3"/>
-    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId4"/>
+    <sheet name="V1.2.4 8_26_2015" sheetId="5" r:id="rId1"/>
+    <sheet name="V1.2.3 7_31_201" sheetId="4" r:id="rId2"/>
+    <sheet name="V1.2.2 7_10_2015" sheetId="3" r:id="rId3"/>
+    <sheet name="V1.2.1 6_9_2015" sheetId="1" r:id="rId4"/>
+    <sheet name="V1.2.0 1_26_2015 (2)" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="41">
   <si>
     <t>Overall Test completion</t>
   </si>
@@ -141,6 +142,19 @@
     <t>Confirm release directory has necessary files   ex: /Users/scoleman/dev/fips/fcids/release/V1.2.0_01_26_2015  Confirm no errors</t>
+  </si>
+  <si>
+    <t>All unit tests pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: This need not be tested unless the t2crypto module has been updated and re-installed in this app:
+    cordova plugin rm org.t2crypto
+    cordova plugin add /Users/scoleman/dev/fips/cordova-plugin-t2crypto
+    cordova build ios
+</t>
+  </si>
+  <si>
+    <t>Overall completion</t>
   </si>
 </sst>
 </file>
@@ -1675,9 +1689,796 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:IV28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="1" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="56.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="42.875" style="1" customWidth="1"/>
+    <col min="12" max="256" width="12.25" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="8" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" ht="20.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" ht="32.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" ht="22.25" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" ht="20.25" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="36.25" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="16">
+      <c r="A14" s="5"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="72">
+      <c r="A15" s="5"/>
+      <c r="B15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="16">
+      <c r="A16" s="5"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+    </row>
+    <row r="19" spans="1:16" s="1" customFormat="1" ht="53" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+    </row>
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+    </row>
+    <row r="22" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+    </row>
+    <row r="23" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+    </row>
+    <row r="24" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+    </row>
+    <row r="25" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+    </row>
+    <row r="26" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+    </row>
+    <row r="27" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+    </row>
+    <row r="28" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A28" s="20"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E6" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
@@ -2292,7 +3093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
@@ -2946,7 +3747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
@@ -3610,7 +4411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>

</xml_diff>